<commit_message>
Add more sample data and pictures
</commit_message>
<xml_diff>
--- a/SampleData/Property_Agent.xlsx
+++ b/SampleData/Property_Agent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioCodeProjects\PropertyHub\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AA1545-F58A-4C5C-A6F6-7B5C8ABC3E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B0B6E8-0684-488C-BC0A-CF14A1378879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28470" yWindow="480" windowWidth="22845" windowHeight="20040" xr2:uid="{3129F6B1-9AEB-43A4-A03B-FC7A4494E4C6}"/>
+    <workbookView xWindow="26250" yWindow="285" windowWidth="25155" windowHeight="20565" xr2:uid="{3129F6B1-9AEB-43A4-A03B-FC7A4494E4C6}"/>
   </bookViews>
   <sheets>
     <sheet name="property" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="145">
   <si>
     <t>MLS</t>
   </si>
@@ -206,6 +206,261 @@
   </si>
   <si>
     <t>A Grande Edwardian with a stately presence ideally and strategically situated steps to everything essential. Renovated and Turnkey just pack your bags and move in. This 3 storey 5 bedroom light filled family home has tons of space and is tastefully renovated throughout. The main floor greets you with a spacious foyer and living area. Relax after a long day in front of the fireplace. Entertain family and guests in the classic dining room that joins the modern renovated kitchen. The gourmet cooks kitchen has a special pantry, a large centre island, a walk out to deck and yard. Just off the kitchen area is a family room or what could become a convenient home office. A modern 4 piece bathroom offers convenience on the main floor. The second floor boasts three large bedrooms, a gorgeous 5 piece bath with separate shower and deep soaking claw foot tub. Enjoy the convenience of a 2nd floor laundry room. The third floor has two large bedrooms. The east facing bedroom has the addition of a large deck that overlooks the city skyline. The basement is mostly finished with several convenient spaces, great ceiling height and complete with a bathroom and laundry area. Find a private east facing garden and garage for up to 2 cars off laneway at rear. **** EXTRAS **** Strength in numbers: 557 &amp; 565 Markham St. are also for sale (MLS). Maximize your economies of scale, or dream bigger and assemble 3 flagship properties in enviable location. Located on a Low-Traffic, Tree-lined, One-way Street. (38103986)</t>
+  </si>
+  <si>
+    <t>Daryl CHARLES King</t>
+  </si>
+  <si>
+    <t>N11608454</t>
+  </si>
+  <si>
+    <t>Detached</t>
+  </si>
+  <si>
+    <t>COLESBROOK ROAD</t>
+  </si>
+  <si>
+    <t>Richmond Hill</t>
+  </si>
+  <si>
+    <t>L4S2G3</t>
+  </si>
+  <si>
+    <t>Beautifully upgraded, 4+1 bedroom family home on quiet street backing onto tranquil walking trail with no neighboursbehind! No expense spared in upgrades inside &amp; out! Above grade, lower level in-law suite/apt with walk-out to private yard, salt-water pool &amp;patio. Open concept main floor features a sunken foyer with soaring ceiling open to above, hardwood floors, 9 ceilings, oak staircase withwrought-iron spindles, LED pot lights, smooth ceilings &amp; custom millwork. Family room features huge windows with automatic blinds, vaultedceiling, gas fireplace &amp; surround sound. The sun-filled main floor is ideal for entertaining and boasts an impressive, Chef inspired kitchen withhigh-end appliances: built-in Bertazzoni fridge, paneled Bosch dishwasher, 6 burner gas range with pot filler/tap &amp; custom range hood, hugeisland with 2-way storage cabinets, double undermount sink &amp; quartz waterfall counter. Extended custom cabinetry, glass display cabinets, 2large pantry cabinets, soft close pot drawers &amp; cabinet doors with soft gold hardware &amp; accents. Kitchen overlooks the open concept living &amp;dining area and has a garden door walkout to a raised private deck complete with gas line for BBQ &amp; automatic awning with remote.Convenient main floor laundry/mud room with direct access to garage, built-in bench, backsplash, quartz counter w/undermount sink &amp;custom cabinetry. Second floor features a spacious primary suite with built-in armoire, walk-in closet with organizers &amp; a 5 pc ensuite. Threeadditional bedrooms are located on the upper level and share a main 4pc bath, all with custom shutters &amp; closet organizers. The lower level isa great space for extended family or older children &amp; features 1 bedroom, 3pc bath, laundry room, cold cellar, built-in cabinets, kitchen &amp;sunny living area with built-in shelves, huge windows &amp; separate entrance. Enjoy your own private backyard oasis with salt water pool, patio &amp;raised deck overlooking lush conservation land &amp; walking trail. **** EXTRAS **** Exterior soffit lights, 3 car parking on driveway, 2 car garage w/cabinet system, two 220V outlets, storage loft &amp; new insulated garage doors. Close to public transit, public &amp; catholic schools, William Harrison Park &amp; Trans Richmond Trail. (39305860)</t>
+  </si>
+  <si>
+    <t>Cynthia Dacosta</t>
+  </si>
+  <si>
+    <t>RE/MAX CROSSROADS REALTY INCORPORATED</t>
+  </si>
+  <si>
+    <t>905-305-0505</t>
+  </si>
+  <si>
+    <t>raka@topremax.ca</t>
+  </si>
+  <si>
+    <t>Woodbine Ave</t>
+  </si>
+  <si>
+    <t>Markham</t>
+  </si>
+  <si>
+    <t>L3R 9Y4</t>
+  </si>
+  <si>
+    <t>N11581343</t>
+  </si>
+  <si>
+    <t>MUMBERSON COURT</t>
+  </si>
+  <si>
+    <t>L6C1Y4</t>
+  </si>
+  <si>
+    <t>Stunning Detached Home In Prestigious Cachet Community. 6 Bedrooms Plus 2 In Bsmt, 6 Bathrooms Plus 2 In Bsmt. 3 Car Garage, 2 Fireplaces, Hardwood Floors Throughout. Gourmet Kitchen, Granite Counter Top, 10' Ceiling On Main Floor, Stone Front And Side, Crown Moulding Throughout, Large Skylight. Sprinkler System, Lot Of Pot Lights, Security System, Cameras, 8' Baseboards, New Roof, Prof Landscaping, Too Many Upgrades To List, Super Condition, 4,300Sqft **** EXTRAS **** Build In Fridge, Dishwasher, Stove, Microwave, Warmer, Washer&amp;Dryer, Lot Of Cabinet Space, All Window Coverings, Elfs , Cac, Cvc, Garage Door Opener And Remote, 4 Web Cameras (Can Be Extended To 8). To Verify All Measurements And Taxes. (39278311)</t>
+  </si>
+  <si>
+    <t>Pepito SUNDIAM Lintag</t>
+  </si>
+  <si>
+    <t>ROYAL LEPAGE SIGNATURE REALTY</t>
+  </si>
+  <si>
+    <t>416-443-0300</t>
+  </si>
+  <si>
+    <t>chris@slightham.com</t>
+  </si>
+  <si>
+    <t>M3C 0H5</t>
+  </si>
+  <si>
+    <t>SAMPSON MEWS</t>
+  </si>
+  <si>
+    <t>E11821382</t>
+  </si>
+  <si>
+    <t>WYPER SQUARE</t>
+  </si>
+  <si>
+    <t>M1S0B3</t>
+  </si>
+  <si>
+    <t>Rare Find At This Location. One Of The Largest House In Highgate Court (2,338 SqFt)! Minutes Walk To Soon To Open Scarborough Subway Extension! Features Lots Of Upgrades 9 Ft Ceiling On Main! Stamp Concrete Driveway, Hardwood Floors All Throughout, Quartz Counters On Kitchen. Short Drive To STC And 401. **** EXTRAS **** S/S Refrigerator, S/S Oven Range, S/S Dishwasher, S/S Range Hood, Washer &amp; Dryer. All Existing Light Fixtures, Garage Door Opener &amp; Remote. Hwt Is Rental (Enercare). (39519714)</t>
+  </si>
+  <si>
+    <t>Hubert Kin Ming Lee</t>
+  </si>
+  <si>
+    <t>LANDPOWER REAL ESTATE LTD.</t>
+  </si>
+  <si>
+    <t>905-305-9669</t>
+  </si>
+  <si>
+    <t>mail@landpower.ca</t>
+  </si>
+  <si>
+    <t>HIGHWAY 7 EAST</t>
+  </si>
+  <si>
+    <t>MARKHAM</t>
+  </si>
+  <si>
+    <t>L3R 0G6</t>
+  </si>
+  <si>
+    <t>C11821862</t>
+  </si>
+  <si>
+    <t>SKYMARK DRIVE</t>
+  </si>
+  <si>
+    <t>M2H3N9</t>
+  </si>
+  <si>
+    <t>*Rarely Oered* Enjoy Breathtaking, Unobstructed Panoramic Views Of Endless Green Landscapes. Oering A Serene EscapeAnd Stunning Vistas In Every Direction. Welcome To The Elegance Built By Tridel. Smart-Size Living At Its Finest. Featuring Two Bedroom AndTwo Full Baths (Majority Of The 07 Units Only Have 1.5 Baths And No Longer Can Add 2nd Full Bath). Modern Kitchen W/ S/S Appliances,Granite Countertops, Pantry, Pot Lights, Under Cabinet Lights, And Breakfast Bar. Experience A Lifestyle Of Luxury With Hotel-Like Amenities:Doorman (Opens Door, Helps With Groceries, Luggage etc), 24/7 Gatehouse, Indoor &amp; Outdoor Pools, Hot Tub, Sauna, Gyms, Billiards, TableTennis, Pickleball, Tennis, Basketball, Squash, Party Room, Library, Private Trail and More! Excellent School Zone: Hillmount PS, Highland MS,AY Jackson. *A Must See* **** EXTRAS **** Internet, TV and Utilities All Included In Condo Fees. 2 Parking Spaces. *EV Charger Available For Purchase Through Mgmt At A LowCost* (39521183)</t>
+  </si>
+  <si>
+    <t>Karyna Gongalskyy</t>
+  </si>
+  <si>
+    <t>ROYAL LEPAGE REALTY PLUS</t>
+  </si>
+  <si>
+    <t>905-828-6550</t>
+  </si>
+  <si>
+    <t>carlo@royallepage.ca</t>
+  </si>
+  <si>
+    <t>DUNDAS STREET WEST</t>
+  </si>
+  <si>
+    <t>MISSISSAUGA</t>
+  </si>
+  <si>
+    <t>L5K 2M6</t>
+  </si>
+  <si>
+    <t>W11821779</t>
+  </si>
+  <si>
+    <t>ELM DRIVE</t>
+  </si>
+  <si>
+    <t>Mississauga</t>
+  </si>
+  <si>
+    <t>L5B1P2</t>
+  </si>
+  <si>
+    <t>Experience unparalleled living in this exquisite, modern corner unit, offering breathtaking and unobstructed views. The expansive master bedroom features an ensuite and a spacious closet, ensuring comfort and convenience. The sleek, contemporary kitchen is equipped with top-of-the-line stainless steel appliances and a built-in island, perfect for culinary enthusiasts. The unit also boasts a large second bedroom, providing ample space for family or guests. Uniquely positioned with the only balcony on the building's side, this residence offers exclusive, unobstructed vistas, creating a serene and private outdoor retreat. Nestled in a prime location, the property is surrounded by an array of shopping destinations and picturesque parks, enhancing the urban living experience. With its combination of modern design, premium amenities, and an enviable location, this unit is a rare find and an absolute must-see. Do not miss the opportunity to make this exceptional residence your new home. (39520985)</t>
+  </si>
+  <si>
+    <t>Mohita Singh</t>
+  </si>
+  <si>
+    <t>HOMELIFE MAPLE LEAF REALTY LTD.</t>
+  </si>
+  <si>
+    <t>905-456-9090</t>
+  </si>
+  <si>
+    <t>office@hlmapleleaf.com</t>
+  </si>
+  <si>
+    <t>EASTERN AVENUE</t>
+  </si>
+  <si>
+    <t>BRAMPTON</t>
+  </si>
+  <si>
+    <t>L6W 1X9</t>
+  </si>
+  <si>
+    <t>W11821602</t>
+  </si>
+  <si>
+    <t>MATAGAMI STREET</t>
+  </si>
+  <si>
+    <t>Brampton</t>
+  </si>
+  <si>
+    <t>L6Y0M9</t>
+  </si>
+  <si>
+    <t>Welcome to this stunning all brick detached 3000 sqft plus, 4 bedroom home with a LEGAL 2 BEDROOM BASEMENT APARTMENT. Clean And Spotless Home in a quiet Neighborhood . Gleaming hardwood Floors throughout. Newer Roof (1 Year).. Newer A/C And Furnace. Upstairs extra office/den area. Oak Staircase Upgraded Stair railing. Upgraded Fireplace &amp; Kitchen. All Washrooms have marble Counters.. Close to all amenities, Banks, Restaurants, Library, Shopping in the newer Plazas on the prestigious Mississauga Road. Close to Highways 407 and 401. Come &amp; See This Beautiful Home Today! (39520417)</t>
+  </si>
+  <si>
+    <t>Changxi Tu</t>
+  </si>
+  <si>
+    <t>HOMELIFE LANDMARK REALTY INC.</t>
+  </si>
+  <si>
+    <t>905-305-1600</t>
+  </si>
+  <si>
+    <t>admin@homelifelandmark.com</t>
+  </si>
+  <si>
+    <t>WOODBINE AVENUE</t>
+  </si>
+  <si>
+    <t>L3R 1A4</t>
+  </si>
+  <si>
+    <t>W11821335</t>
+  </si>
+  <si>
+    <t>DRYSDALE CRESCENT</t>
+  </si>
+  <si>
+    <t>Milton</t>
+  </si>
+  <si>
+    <t>L9T8J2</t>
+  </si>
+  <si>
+    <t>4 Bedroom Detached Home In Highly Desired Willmott Neighborhood. Newly Painted, Open Concept Layout, Plenty Of Pot Lights, 9 Ft Ceiling &amp; Hardwood Flooring On Main Level, Crown Moulding Throughout, California Shutters For All Windows, Upgraded Kitchen With Island/Breakfast Bar/Granite countertops/Stainless Steels Appliances(Gas Stove), Large Master Br With 5 Pcs Ensuite &amp; Walk-in Closet, All Other Three Bedrooms Are Good Size With Large Window/Closet, Fully Fenced Backyard With A Large Deck, Conveniently Located Close To Shopping Plaza, Community Centre, Hospital, Parks, Schools, Milton GO Station And More. **** EXTRAS **** All Existing: Fridge, Stove, Range Hood, Dishwasher, Washer &amp; Dryer, Electric Light Fixtures, Window Coverings, central vacuum. (39519611)</t>
+  </si>
+  <si>
+    <t>Damiris Moro</t>
+  </si>
+  <si>
+    <t>RE/MAX WEST REALTY INC.</t>
+  </si>
+  <si>
+    <t>416-745-2300</t>
+  </si>
+  <si>
+    <t>jcolatosti@remaxwest.net</t>
+  </si>
+  <si>
+    <t>REXDALE BOULEVARD</t>
+  </si>
+  <si>
+    <t>M9W 1N7</t>
+  </si>
+  <si>
+    <t>N11443752</t>
+  </si>
+  <si>
+    <t>FOREST GROVE COURT</t>
+  </si>
+  <si>
+    <t>Aurora</t>
+  </si>
+  <si>
+    <t>L4G3G4</t>
+  </si>
+  <si>
+    <t>Outstanding 5 Bedroom, 5 Bathroom, Executive 4300 + sqft home. On A Private Enclave In A Prestigious Neighborhood of Aurora. Situated On A Child Safe Court With A Rare 59 ft Frontage, Backs onto a protected forest with a park nearby. The Open Concept professionally finished basement with a separate theatre, exercise and games area, also has a kitchenette, powder room large enough to install a shower and ample storage space. Adding another 1800 sqft of luxury, comfort, and elegance to this exquisite home. $300k was spent in upgrades, renovations and improvements. The custom kitchen with integrated high-end appliances, recess lighting, extra cabinetry, quartz counter, large center island plus a breakfast area is a dream for any chef. Coupled with the stunning family room with its marble wall, built-in cabinets, gas fireplace, huge picture window and walk-out to treed serene backyard, It becomes a focal point *the heart of the home* perfect for entertaining and family gatherings. Primary bedroom is large enough for sitting area, walk-in closet and 5 pc spa ensuite. The rest of the bedrooms are spacious and share 2 semi ensuite, a bonus is the den on the second floor. Don't Miss Out! Definitely an Exceptional Property in a premier location, close to 404, private schools, golf course, big box stores, 10min to the Go Station and boutique shopping. A Gem! **** EXTRAS **** Intergraded high end appliances, pot lights thru out, high baseboards, marble fireplace wall, with built-in cabinets, designer like fixtures, front and back landscaping, smooth sailings, soft-water system, accent wall paneling. (39137225)</t>
   </si>
 </sst>
 </file>
@@ -573,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED58E987-85A3-456C-B53A-6FA6B48DDB65}">
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,6 +1052,556 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1899000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2005</v>
+      </c>
+      <c r="I4" s="1">
+        <v>7381.25</v>
+      </c>
+      <c r="J4" s="1">
+        <v>106</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S4" s="1">
+        <v>2836408</v>
+      </c>
+      <c r="U4" s="1">
+        <v>7</v>
+      </c>
+      <c r="V4" s="1">
+        <v>6</v>
+      </c>
+      <c r="W4" s="1">
+        <v>6</v>
+      </c>
+      <c r="X4" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2488800</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1998</v>
+      </c>
+      <c r="I5" s="1">
+        <v>11738.66</v>
+      </c>
+      <c r="J5" s="1">
+        <v>2</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="S5" s="1">
+        <v>2622753</v>
+      </c>
+      <c r="U5" s="1">
+        <v>8</v>
+      </c>
+      <c r="V5" s="1">
+        <v>7</v>
+      </c>
+      <c r="W5" s="1">
+        <v>7</v>
+      </c>
+      <c r="X5" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="1">
+        <v>998800</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1800</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5800.99</v>
+      </c>
+      <c r="J6" s="1">
+        <v>54</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S6" s="1">
+        <v>4723753</v>
+      </c>
+      <c r="U6" s="1">
+        <v>5</v>
+      </c>
+      <c r="V6" s="1">
+        <v>5</v>
+      </c>
+      <c r="W6" s="1">
+        <v>6</v>
+      </c>
+      <c r="X6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1048000</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1600</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2008</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3032.82</v>
+      </c>
+      <c r="J7" s="1">
+        <v>65</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L7" s="1">
+        <v>2307</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S7" s="1">
+        <v>5018980</v>
+      </c>
+      <c r="U7" s="1">
+        <v>8</v>
+      </c>
+      <c r="V7" s="1">
+        <v>8</v>
+      </c>
+      <c r="W7" s="1">
+        <v>9</v>
+      </c>
+      <c r="X7" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1">
+        <v>749000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>856</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2012</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3900</v>
+      </c>
+      <c r="J8" s="1">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L8" s="1">
+        <v>3408</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S8" s="1">
+        <v>4771736</v>
+      </c>
+      <c r="U8" s="1">
+        <v>7</v>
+      </c>
+      <c r="V8" s="1">
+        <v>6</v>
+      </c>
+      <c r="W8" s="1">
+        <v>5</v>
+      </c>
+      <c r="X8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1589000</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3200</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2013</v>
+      </c>
+      <c r="I9" s="1">
+        <v>7566.27</v>
+      </c>
+      <c r="J9" s="1">
+        <v>17</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="S9" s="1">
+        <v>4752028</v>
+      </c>
+      <c r="U9" s="1">
+        <v>6</v>
+      </c>
+      <c r="V9" s="1">
+        <v>3</v>
+      </c>
+      <c r="W9" s="1">
+        <v>7</v>
+      </c>
+      <c r="X9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1380000</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2800</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2015</v>
+      </c>
+      <c r="I10" s="1">
+        <v>5398</v>
+      </c>
+      <c r="J10" s="1">
+        <v>942</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="S10" s="1">
+        <v>4746780</v>
+      </c>
+      <c r="U10" s="1">
+        <v>5</v>
+      </c>
+      <c r="V10" s="1">
+        <v>2</v>
+      </c>
+      <c r="W10" s="1">
+        <v>3</v>
+      </c>
+      <c r="X10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2850000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3800</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I11" s="1">
+        <v>10566</v>
+      </c>
+      <c r="J11" s="1">
+        <v>6</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="S11" s="1">
+        <v>1435803</v>
+      </c>
+      <c r="U11" s="1">
+        <v>6</v>
+      </c>
+      <c r="V11" s="1">
+        <v>6</v>
+      </c>
+      <c r="W11" s="1">
+        <v>7</v>
+      </c>
+      <c r="X11" s="1">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -805,16 +1610,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1229DD12-2EB2-4255-B3F7-61F86A5983B5}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -946,10 +1751,340 @@
         <v>36</v>
       </c>
     </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2836408</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="1">
+        <v>630</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2622753</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="1">
+        <v>8901</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="1">
+        <v>208</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4723753</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="1">
+        <v>8</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="1">
+        <v>201</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5018980</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3621</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="1">
+        <v>403</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>4771736</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2575</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="1">
+        <v>13</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4752028</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="1">
+        <v>80</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>4746780</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="1">
+        <v>7240</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" s="1">
+        <v>103</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1435803</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G11" s="1">
+        <v>96</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{F844F1BB-8C0B-40B2-9B2C-BBFC45253FE7}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{30D88302-70D7-4EF8-9073-2A64935EBAA3}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{349AA53C-355D-4BA3-B2C6-76CE9A462F40}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{B913DCEF-45AC-4FCB-89BD-476D11893681}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{8D3E7291-D8D6-4016-A0AB-9D18176587D5}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{66F086A6-0EE6-410F-BE91-2D7C80E28D43}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{0456398B-0815-400F-875E-EA40E415ADED}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{67518D90-1077-459A-82B3-09377ABF5B85}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{60AF32C8-732F-4EAA-BCDA-1D1F0BF71703}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{413D57AD-D38F-467E-BEC2-5F6224F8F13C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>